<commit_message>
Add problem statement and solutions for identifying missing invoice serial numbers
</commit_message>
<xml_diff>
--- a/Find_Missing_Data/Problem_Statement.xlsx
+++ b/Find_Missing_Data/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q14/Video_Q14_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Find_Missing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09FE957-7D53-C843-A7F0-2463C041DF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EF3132-D26A-424B-AA86-C4F603965345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{41207210-82F9-DE41-B5F0-56CD4CB4D823}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{41207210-82F9-DE41-B5F0-56CD4CB4D823}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,29 +49,6 @@
   </si>
   <si>
     <t>MISSING_SERIAL_NO</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Video #14</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Find missing data</t>
-    </r>
   </si>
   <si>
     <r>
@@ -106,6 +81,29 @@
       </rPr>
       <t>In the given input table, some of the invoice are missing, write a sql query to identify the missing serial no. 
 As an assumption, consider the serial no with the lowest value to be the first generated invoice and the highest serial no value to be the last generated invoice</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Find missing data</t>
     </r>
   </si>
 </sst>
@@ -439,42 +437,42 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,141 +810,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70FD00C-E9CE-E840-B83D-97D3EC72C5A2}">
   <dimension ref="B1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="4" width="15.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="20.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="4" width="15.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="20.796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="15" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:6" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="2:6" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="18"/>
+      <c r="F7" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>330115</v>
       </c>
       <c r="C9" s="7">
         <v>45352</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="F9" s="18">
+      <c r="D9" s="13"/>
+      <c r="F9" s="14">
         <v>330116</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>330120</v>
       </c>
       <c r="C10" s="3">
         <v>45352</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="F10" s="19">
+      <c r="D10" s="13"/>
+      <c r="F10" s="15">
         <v>330117</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>330121</v>
       </c>
       <c r="C11" s="3">
         <v>45352</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="F11" s="19">
+      <c r="D11" s="13"/>
+      <c r="F11" s="15">
         <v>330118</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>330122</v>
       </c>
       <c r="C12" s="3">
         <v>45353</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="F12" s="19">
+      <c r="D12" s="13"/>
+      <c r="F12" s="15">
         <v>330119</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>330125</v>
       </c>
       <c r="C13" s="5">
         <v>45353</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="F13" s="19">
+      <c r="D13" s="13"/>
+      <c r="F13" s="15">
         <v>330123</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="20">
+    <row r="14" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="16">
         <v>330124</v>
       </c>
     </row>
@@ -957,5 +955,6 @@
     <mergeCell ref="B2:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>